<commit_message>
Add more beneficiary fields to bulk upload
</commit_message>
<xml_diff>
--- a/web-app/secured/ProjectsUploadTemplate.xlsx
+++ b/web-app/secured/ProjectsUploadTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="28220" windowHeight="17000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>amount</t>
   </si>
@@ -146,6 +146,57 @@
   </si>
   <si>
     <t>createdDate</t>
+  </si>
+  <si>
+    <t>telephone</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>addressLine1</t>
+  </si>
+  <si>
+    <t>addressLine2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>stateOrProvince</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>91 (80) 26677444</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>UNSPECIFIED</t>
+  </si>
+  <si>
+    <t>123 Sample Street</t>
+  </si>
+  <si>
+    <t>Basavanagudi</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -609,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="O1" sqref="O1:V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -624,7 +675,7 @@
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -666,6 +717,30 @@
       </c>
       <c r="N1" t="s">
         <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -681,10 +756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:N2"/>
+      <selection sqref="A1:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -694,9 +769,10 @@
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -739,8 +815,32 @@
       <c r="N1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="2">
         <v>41654</v>
       </c>
@@ -783,8 +883,32 @@
       <c r="N2" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2">
+        <v>560028</v>
+      </c>
+      <c r="V2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
@@ -797,8 +921,11 @@
       <c r="K5" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="P5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="D6" t="s">
         <v>3</v>
       </c>
@@ -811,8 +938,11 @@
       <c r="K6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="P6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -822,16 +952,22 @@
       <c r="F7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="P7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="D8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="P8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="D9" t="s">
         <v>7</v>
       </c>
@@ -839,7 +975,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:22">
       <c r="D10" t="s">
         <v>8</v>
       </c>
@@ -847,7 +983,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:22">
       <c r="D11" t="s">
         <v>9</v>
       </c>
@@ -855,27 +991,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:22">
       <c r="F12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:22">
       <c r="F13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:22">
       <c r="F14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:22">
       <c r="F15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:22">
       <c r="F16" t="s">
         <v>11</v>
       </c>
@@ -885,6 +1021,7 @@
     <hyperlink ref="N2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>